<commit_message>
chore: wall terminals 6 and 8
</commit_message>
<xml_diff>
--- a/docs/Mappa zone (compilato).xlsx
+++ b/docs/Mappa zone (compilato).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Domoticata\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CA0246-F3A7-4874-BEA6-3C0F6A341808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDAD76F-2877-4AFA-9A0E-D642F1EC7674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2471F9E7-F142-4FD4-B46F-4DD068C747A6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="18">
   <si>
     <t>Zona</t>
   </si>
@@ -317,7 +317,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -365,15 +365,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -715,7 +706,7 @@
   <dimension ref="B2:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20:H20"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,7 +769,7 @@
       <c r="J3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="17">
+      <c r="K3" s="15">
         <v>10</v>
       </c>
       <c r="L3" s="16"/>
@@ -805,7 +796,7 @@
       <c r="J4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="2">
         <v>7</v>
       </c>
       <c r="L4" s="11" t="s">
@@ -830,7 +821,7 @@
       <c r="J5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="19"/>
+      <c r="K5" s="5"/>
       <c r="L5" s="12"/>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
@@ -847,7 +838,7 @@
       <c r="J6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="19"/>
+      <c r="K6" s="5"/>
       <c r="L6" s="12"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
@@ -893,7 +884,7 @@
       <c r="J8" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K8" s="17">
+      <c r="K8" s="15">
         <v>11</v>
       </c>
       <c r="L8" s="16"/>
@@ -920,7 +911,7 @@
       <c r="J9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="2">
         <v>1</v>
       </c>
       <c r="L9" s="11" t="s">
@@ -949,7 +940,7 @@
       <c r="J10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="18">
+      <c r="K10" s="2">
         <v>2</v>
       </c>
       <c r="L10" s="11" t="s">
@@ -970,7 +961,7 @@
       <c r="J11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K11" s="18">
+      <c r="K11" s="2">
         <v>4</v>
       </c>
       <c r="L11" s="11" t="s">
@@ -990,12 +981,8 @@
       <c r="F12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G12" s="4">
-        <v>8</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>16</v>
-      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="13"/>
       <c r="J12" s="3" t="s">
         <v>4</v>
       </c>
@@ -1024,7 +1011,7 @@
       <c r="J13" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K13" s="17">
+      <c r="K13" s="15">
         <v>12</v>
       </c>
       <c r="L13" s="16"/>
@@ -1051,7 +1038,7 @@
       <c r="J14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K14" s="18">
+      <c r="K14" s="2">
         <v>6</v>
       </c>
       <c r="L14" s="11" t="s">
@@ -1076,7 +1063,7 @@
       <c r="J15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K15" s="19"/>
+      <c r="K15" s="5"/>
       <c r="L15" s="12"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
@@ -1093,7 +1080,7 @@
       <c r="J16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K16" s="19"/>
+      <c r="K16" s="5"/>
       <c r="L16" s="12"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
@@ -1198,12 +1185,8 @@
       <c r="F22" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G22" s="4">
-        <v>7</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>15</v>
-      </c>
+      <c r="G22" s="6"/>
+      <c r="H22" s="13"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">

</xml_diff>